<commit_message>
Add The Day needs
</commit_message>
<xml_diff>
--- a/2020/Work.xlsx
+++ b/2020/Work.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Hall-of-FAME-and-SHAME\2020\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hall-of-FAME-and-SHAME\2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8492F84D-3B00-445D-8FC7-078C5C41167D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5570E48C-2F28-4F6E-A68F-2C5D6D0D9845}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{69693E65-AD6F-44D6-B0ED-1B386BB2E7FA}"/>
   </bookViews>
@@ -20,18 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>date</t>
   </si>
@@ -103,13 +97,25 @@
   </si>
   <si>
     <t>Review GP</t>
+  </si>
+  <si>
+    <t>Quraan 2 Quarters</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>Bdaya Website Modifications</t>
+  </si>
+  <si>
+    <t>QBS System Work</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,6 +126,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -152,7 +164,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -161,6 +173,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
@@ -476,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DA183D7-129D-4FE3-AEAC-265A19317476}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -601,11 +617,83 @@
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
     </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="4">
+        <f>DATE(2020,10,16)</f>
+        <v>44120</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="5">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="3"/>
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="3"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="3"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="3"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="3"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="4">
+        <f>DATE(2020,10,17)</f>
+        <v>44121</v>
+      </c>
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="5">
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="3"/>
+      <c r="B21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="5">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="3"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="3"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="3"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="3"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="A8:A13"/>
+    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="A20:A25"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding The Day Work
</commit_message>
<xml_diff>
--- a/2020/Work.xlsx
+++ b/2020/Work.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hall-of-FAME-and-SHAME\2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5570E48C-2F28-4F6E-A68F-2C5D6D0D9845}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C85C68BA-EDD4-4343-A8B8-A12D00BD3539}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{69693E65-AD6F-44D6-B0ED-1B386BB2E7FA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
   <si>
     <t>date</t>
   </si>
@@ -109,6 +109,33 @@
   </si>
   <si>
     <t>QBS System Work</t>
+  </si>
+  <si>
+    <t>Radiante ApI working</t>
+  </si>
+  <si>
+    <t>9:00:00 PM : 11:00 PM</t>
+  </si>
+  <si>
+    <t>Fajr</t>
+  </si>
+  <si>
+    <t>4:30/5:00</t>
+  </si>
+  <si>
+    <t>5:30/7:00</t>
+  </si>
+  <si>
+    <t>Travelling</t>
+  </si>
+  <si>
+    <t>7:00/9:00</t>
+  </si>
+  <si>
+    <t>9:00/11:40</t>
+  </si>
+  <si>
+    <t>Duhr</t>
   </si>
 </sst>
 </file>
@@ -170,13 +197,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
@@ -492,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DA183D7-129D-4FE3-AEAC-265A19317476}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -524,7 +551,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
@@ -541,7 +568,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
+      <c r="A3" s="4"/>
       <c r="B3" t="s">
         <v>8</v>
       </c>
@@ -550,7 +577,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
+      <c r="A4" s="4"/>
       <c r="B4" t="s">
         <v>10</v>
       </c>
@@ -559,7 +586,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
+      <c r="A5" s="4"/>
       <c r="B5" t="s">
         <v>13</v>
       </c>
@@ -568,7 +595,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
+      <c r="A6" s="4"/>
       <c r="B6" t="s">
         <v>16</v>
       </c>
@@ -580,10 +607,10 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
+      <c r="A7" s="4"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B8" t="s">
@@ -591,41 +618,41 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
+      <c r="A9" s="4"/>
       <c r="B9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="3"/>
+      <c r="A10" s="4"/>
       <c r="B10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="3"/>
+      <c r="A11" s="4"/>
       <c r="B11" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="3"/>
+      <c r="A12" s="4"/>
       <c r="B12" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="3"/>
+      <c r="A13" s="4"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="4">
+      <c r="A14" s="5">
         <f>DATE(2020,10,16)</f>
         <v>44120</v>
       </c>
       <c r="B14" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="3">
         <v>0.91666666666666663</v>
       </c>
       <c r="D14" t="s">
@@ -633,65 +660,173 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="3"/>
+      <c r="A15" s="4"/>
       <c r="B15" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="3">
         <v>0.5</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="3"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="3"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="3"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="3"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="4">
+      <c r="A16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="4"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="4"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="5">
         <f>DATE(2020,10,17)</f>
         <v>44121</v>
       </c>
       <c r="B20" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="3">
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="3"/>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="4"/>
       <c r="B21" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="3">
         <v>0.375</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="3"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="3"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="3"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="3"/>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="4"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="4"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="4"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="4"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="5">
+        <f>DATE(2020,11,27)</f>
+        <v>44162</v>
+      </c>
+      <c r="B26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="4"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="4"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="4"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="4"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="4"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="5">
+        <f>DATE(2020,11,29)</f>
+        <v>44164</v>
+      </c>
+      <c r="B32" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="4"/>
+      <c r="B33" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="4"/>
+      <c r="B34" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="4"/>
+      <c r="B35" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="4"/>
+      <c r="B36" t="s">
+        <v>28</v>
+      </c>
+      <c r="C36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="4"/>
+      <c r="B37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="5">
+        <f>DATE(2020,11,29)</f>
+        <v>44164</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="4"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="4"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="4"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="4"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="7">
+    <mergeCell ref="A32:A37"/>
+    <mergeCell ref="A38:A43"/>
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="A8:A13"/>
     <mergeCell ref="A14:A19"/>
     <mergeCell ref="A20:A25"/>
+    <mergeCell ref="A26:A31"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>